<commit_message>
Test additional batch processing workflows
</commit_message>
<xml_diff>
--- a/doc/processing_methods.xlsx
+++ b/doc/processing_methods.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="37">
   <si>
     <t>Filter</t>
   </si>
@@ -169,6 +169,16 @@
   </si>
   <si>
     <t>sbe19plus_v2_3</t>
+  </si>
+  <si>
+    <t>Temperature = +0.50
+Conductivity = +0.05</t>
+  </si>
+  <si>
+    <t>sbe19plus_v2_4</t>
+  </si>
+  <si>
+    <t>sbe19plus_v2_5</t>
   </si>
 </sst>
 </file>
@@ -501,19 +511,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="25.26953125" customWidth="1"/>
-    <col min="3" max="10" width="25.90625" customWidth="1"/>
+    <col min="3" max="12" width="25.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>9</v>
       </c>
@@ -533,16 +543,22 @@
         <v>33</v>
       </c>
       <c r="H1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1" t="s">
         <v>12</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>13</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -570,11 +586,17 @@
       <c r="I2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="L2" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="47.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" ht="47.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -602,11 +624,17 @@
       <c r="I3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="J3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="L3" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>17</v>
       </c>
@@ -629,16 +657,22 @@
         <v>24</v>
       </c>
       <c r="H4" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J4" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="K4" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="L4" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
@@ -666,11 +700,17 @@
       <c r="I5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="J5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L5" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -684,10 +724,10 @@
         <v>29</v>
       </c>
       <c r="E6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>19</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>29</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>29</v>
@@ -701,8 +741,14 @@
       <c r="J6" s="3" t="s">
         <v>29</v>
       </c>
+      <c r="K6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
@@ -730,11 +776,17 @@
       <c r="I7" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="J7" s="3" t="s">
         <v>20</v>
       </c>
+      <c r="K7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
@@ -762,11 +814,17 @@
       <c r="I8" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="J8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="L8" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="32" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" ht="32" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
@@ -794,11 +852,17 @@
       <c r="I9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J9" s="1" t="s">
+      <c r="J9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="L9" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -826,7 +890,13 @@
       <c r="I10" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="J10" s="1" t="s">
+      <c r="J10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L10" s="1" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>